<commit_message>
Update the code - class
</commit_message>
<xml_diff>
--- a/script/beta_meta_script/output/meta_output.xlsx
+++ b/script/beta_meta_script/output/meta_output.xlsx
@@ -513,19 +513,19 @@
         <v>0.3711569546144358</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04609949905012686</v>
+        <v>0.04609949905012687</v>
       </c>
       <c r="H2" t="n">
-        <v>8.19764612355504e-16</v>
+        <v>8.197646123555103e-16</v>
       </c>
       <c r="I2" t="n">
-        <v>8.19764612355504e-16</v>
+        <v>8.197646123555103e-16</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0825977170435549</v>
+        <v>0.08259771704355461</v>
       </c>
     </row>
     <row r="3">
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.3714916289836938</v>
+        <v>0.3714916289836939</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05610342297601253</v>
+        <v>0.05610342297601254</v>
       </c>
       <c r="H4" t="n">
         <v>3.554513795792875e-11</v>
@@ -639,19 +639,19 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.5325639672023214</v>
+        <v>0.5325639672023215</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1386793944391461</v>
+        <v>0.138679394439146</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0001229075551679799</v>
+        <v>0.0001229075551679792</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0003687226655039398</v>
+        <v>0.0003687226655039377</v>
       </c>
       <c r="J5" t="n">
-        <v>21.12092752732361</v>
+        <v>21.12092752732359</v>
       </c>
       <c r="K5" t="n">
         <v>1.267763385968311</v>
@@ -682,22 +682,22 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.6437238974622097</v>
+        <v>0.6437238974622098</v>
       </c>
       <c r="G6" t="n">
         <v>0.1713478355518122</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001720824829622887</v>
+        <v>0.0001720824829622885</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0002581237244434331</v>
+        <v>0.0002581237244434327</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05918222103168087</v>
+        <v>0.05918222103168103</v>
       </c>
     </row>
     <row r="7">
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.3354179770700447</v>
+        <v>0.3354179770700445</v>
       </c>
       <c r="G7" t="n">
         <v>0.1311381600434696</v>
@@ -737,10 +737,10 @@
         <v>0.01053533065459248</v>
       </c>
       <c r="J7" t="n">
-        <v>50.72911937243612</v>
+        <v>50.72911937243607</v>
       </c>
       <c r="K7" t="n">
-        <v>2.029596360493229</v>
+        <v>2.029596360493227</v>
       </c>
     </row>
     <row r="8">
@@ -814,13 +814,13 @@
         <v>-0.3513041745623368</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03136179445042606</v>
+        <v>0.03136179445042608</v>
       </c>
       <c r="H9" t="n">
-        <v>4.001616775551876e-29</v>
+        <v>4.001616775552105e-29</v>
       </c>
       <c r="I9" t="n">
-        <v>8.003233551103753e-29</v>
+        <v>8.00323355110421e-29</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -857,19 +857,19 @@
         <v>-0.292415627494133</v>
       </c>
       <c r="G10" t="n">
-        <v>0.07117159234968994</v>
+        <v>0.07117159234968995</v>
       </c>
       <c r="H10" t="n">
-        <v>3.980642766046332e-05</v>
+        <v>3.980642766046361e-05</v>
       </c>
       <c r="I10" t="n">
-        <v>3.980642766046332e-05</v>
+        <v>3.980642766046361e-05</v>
       </c>
       <c r="J10" t="n">
-        <v>0.8637496248891832</v>
+        <v>0.8637496248891177</v>
       </c>
       <c r="K10" t="n">
-        <v>1.008712752616938</v>
+        <v>1.008712752616937</v>
       </c>
     </row>
     <row r="11">
@@ -900,19 +900,19 @@
         <v>0.3403853571739563</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0893280469126957</v>
+        <v>0.08932804691269569</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0001386807718349997</v>
+        <v>0.000138680771834999</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0001386807718349997</v>
+        <v>0.000138680771834999</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.001571401341456814</v>
+        <v>0.00157140134145679</v>
       </c>
     </row>
     <row r="12">
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.2662021511122399</v>
+        <v>0.2662021511122402</v>
       </c>
     </row>
     <row r="13">
@@ -1026,22 +1026,22 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.2140221834170826</v>
+        <v>0.2140221834170827</v>
       </c>
       <c r="G14" t="n">
-        <v>0.02779625919193586</v>
+        <v>0.02779625919193585</v>
       </c>
       <c r="H14" t="n">
-        <v>1.364119110844801e-14</v>
+        <v>1.364119110844762e-14</v>
       </c>
       <c r="I14" t="n">
-        <v>1.364119110844801e-14</v>
+        <v>1.364119110844762e-14</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.6794490340344341</v>
+        <v>0.6794490340344336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>